<commit_message>
new code by swetha
</commit_message>
<xml_diff>
--- a/src/test/resources/database/TestData.xlsx
+++ b/src/test/resources/database/TestData.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Vulcan_GroupActivity\VULCUAN_Cucumber_Framework\src\test\resources\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Swetha\VULCUAN_Cucumber_Framework\VULCUAN_Cucumber_Framework\src\test\resources\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BA3AE3-1F60-4C59-88D4-0423B75B55E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59EF191-622E-4D73-94B5-459F17B53EBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="2175" windowWidth="19920" windowHeight="7110" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="1170" windowWidth="19920" windowHeight="7110" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="DomesticFTA" sheetId="2" r:id="rId2"/>
+    <sheet name="InternationalFT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>S.No</t>
   </si>
@@ -515,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E91CADB-E8C6-4F66-A885-A40DC0D6E630}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,4 +706,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7776799E-0F75-4278-ACA3-2233F84FA8C8}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>1234556657</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2">
+        <v>120481</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>